<commit_message>
Excel ready, waiting update
</commit_message>
<xml_diff>
--- a/jane/jane_metadata.xlsx
+++ b/jane/jane_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eck44\IntarsiaHtml\IntarsiaPortfolio\jane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F82DC0AA-6383-44E8-ACBB-16F0DC8DE092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08F0D651-474D-43A1-8A8D-19F1D2CFB09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1680" windowWidth="29040" windowHeight="15720" xr2:uid="{EE04B4BD-73DE-4B61-9F4B-7724C0642952}"/>
+    <workbookView xWindow="-28920" yWindow="-1680" windowWidth="29040" windowHeight="15720" xr2:uid="{B3066F03-A37A-4719-80B8-1FB60586D500}"/>
   </bookViews>
   <sheets>
     <sheet name="jane_metadata" sheetId="1" r:id="rId1"/>
@@ -154,190 +154,190 @@
     <t>Giraffequilt</t>
   </si>
   <si>
+    <t>HarryPotterquilt.jpg</t>
+  </si>
+  <si>
+    <t>Harrypotterquilt</t>
+  </si>
+  <si>
+    <t>Heartquilt.JPG</t>
+  </si>
+  <si>
+    <t>Heartquilt</t>
+  </si>
+  <si>
+    <t>HummingbirdLegitKits.jpg</t>
+  </si>
+  <si>
+    <t>Hummingbirdlegitkits</t>
+  </si>
+  <si>
+    <t>Irisblockquilt.JPG</t>
+  </si>
+  <si>
+    <t>Irisblockquilt</t>
+  </si>
+  <si>
+    <t>Irishchain.jpg</t>
+  </si>
+  <si>
+    <t>Irishchain</t>
+  </si>
+  <si>
+    <t>JNeimeyerQuilt.jpg</t>
+  </si>
+  <si>
+    <t>Jneimeyerquilt</t>
+  </si>
+  <si>
+    <t>JudyNeimeyerquilt2.jpg</t>
+  </si>
+  <si>
+    <t>Judyneimeyerquilt2</t>
+  </si>
+  <si>
+    <t>JudyNeimyer1stquilt.jpg</t>
+  </si>
+  <si>
+    <t>Judyneimyer1Stquilt</t>
+  </si>
+  <si>
+    <t>KamalaHarris.jpg</t>
+  </si>
+  <si>
+    <t>Kamalaharris</t>
+  </si>
+  <si>
+    <t>MHPXE4909.JPG</t>
+  </si>
+  <si>
+    <t>Mhpxe4909</t>
+  </si>
+  <si>
+    <t>OneBlockwonder2025.jpg</t>
+  </si>
+  <si>
+    <t>Oneblockwonder2025</t>
+  </si>
+  <si>
+    <t>OpticalIllusianQuilt.jpg</t>
+  </si>
+  <si>
+    <t>Opticalillusianquilt</t>
+  </si>
+  <si>
+    <t>OrchidThreadPainting.JPG</t>
+  </si>
+  <si>
+    <t>Orchidthreadpainting</t>
+  </si>
+  <si>
+    <t>Owl.jpg</t>
+  </si>
+  <si>
+    <t>Owl</t>
+  </si>
+  <si>
+    <t>PeanutsRaffle.png</t>
+  </si>
+  <si>
+    <t>Peanutsraffle</t>
+  </si>
+  <si>
+    <t>Playbillquilt.JPG</t>
+  </si>
+  <si>
+    <t>Playbillquilt</t>
+  </si>
+  <si>
+    <t>Playbillquilt2.JPG</t>
+  </si>
+  <si>
+    <t>Playbillquilt2</t>
+  </si>
+  <si>
+    <t>PortraitquiltMom.JPG</t>
+  </si>
+  <si>
+    <t>Portraitquiltmom</t>
+  </si>
+  <si>
+    <t>Ratatouillequilt.jpg</t>
+  </si>
+  <si>
+    <t>Ratatouillequilt</t>
+  </si>
+  <si>
+    <t>RileyCummingsgift2010.jpg</t>
+  </si>
+  <si>
+    <t>Rileycummingsgift2010</t>
+  </si>
+  <si>
+    <t>SamMinsleyMSUquilt2025.jpg</t>
+  </si>
+  <si>
+    <t>Samminsleymsuquilt2025</t>
+  </si>
+  <si>
+    <t>SesameStreetquilt.jpg</t>
+  </si>
+  <si>
+    <t>Sesamestreetquilt</t>
+  </si>
+  <si>
+    <t>StarTreckquilt.JPG</t>
+  </si>
+  <si>
+    <t>Startreckquilt</t>
+  </si>
+  <si>
+    <t>StarTrekquilt.jpg</t>
+  </si>
+  <si>
+    <t>Startrekquilt</t>
+  </si>
+  <si>
+    <t>Sunflowerqult.jpg</t>
+  </si>
+  <si>
+    <t>Sunflowerqult</t>
+  </si>
+  <si>
+    <t>Tablerunner.JPG</t>
+  </si>
+  <si>
+    <t>Tablerunner</t>
+  </si>
+  <si>
+    <t>TheVeryHungryCaterpillar.jpg</t>
+  </si>
+  <si>
+    <t>Theveryhungrycaterpillar</t>
+  </si>
+  <si>
+    <t>TropicalBirds.JPG</t>
+  </si>
+  <si>
+    <t>Tropicalbirds</t>
+  </si>
+  <si>
+    <t>Tshirtquilt for ADA.JPG</t>
+  </si>
+  <si>
+    <t>Tshirtquilt For Ada</t>
+  </si>
+  <si>
+    <t>Zebraqult.JPG</t>
+  </si>
+  <si>
+    <t>Zebraqult</t>
+  </si>
+  <si>
     <t>HarryPotterquilt2.JPG</t>
   </si>
   <si>
     <t>Harrypotterquilt2</t>
-  </si>
-  <si>
-    <t>HarryPotterquilt.jpg</t>
-  </si>
-  <si>
-    <t>Harrypotterquilt</t>
-  </si>
-  <si>
-    <t>Heartquilt.JPG</t>
-  </si>
-  <si>
-    <t>Heartquilt</t>
-  </si>
-  <si>
-    <t>HummingbirdLegitKits.jpg</t>
-  </si>
-  <si>
-    <t>Hummingbirdlegitkits</t>
-  </si>
-  <si>
-    <t>Irisblockquilt.JPG</t>
-  </si>
-  <si>
-    <t>Irisblockquilt</t>
-  </si>
-  <si>
-    <t>Irishchain.jpg</t>
-  </si>
-  <si>
-    <t>Irishchain</t>
-  </si>
-  <si>
-    <t>JNeimeyerQuilt.jpg</t>
-  </si>
-  <si>
-    <t>Jneimeyerquilt</t>
-  </si>
-  <si>
-    <t>JudyNeimeyerquilt2.jpg</t>
-  </si>
-  <si>
-    <t>Judyneimeyerquilt2</t>
-  </si>
-  <si>
-    <t>JudyNeimyer1stquilt.jpg</t>
-  </si>
-  <si>
-    <t>Judyneimyer1Stquilt</t>
-  </si>
-  <si>
-    <t>KamalaHarris.jpg</t>
-  </si>
-  <si>
-    <t>Kamalaharris</t>
-  </si>
-  <si>
-    <t>MHPXE4909.JPG</t>
-  </si>
-  <si>
-    <t>Mhpxe4909</t>
-  </si>
-  <si>
-    <t>OneBlockwonder2025.jpg</t>
-  </si>
-  <si>
-    <t>Oneblockwonder2025</t>
-  </si>
-  <si>
-    <t>OpticalIllusianQuilt.jpg</t>
-  </si>
-  <si>
-    <t>Opticalillusianquilt</t>
-  </si>
-  <si>
-    <t>OrchidThreadPainting.JPG</t>
-  </si>
-  <si>
-    <t>Orchidthreadpainting</t>
-  </si>
-  <si>
-    <t>Owl.jpg</t>
-  </si>
-  <si>
-    <t>Owl</t>
-  </si>
-  <si>
-    <t>PeanutsRaffle.png</t>
-  </si>
-  <si>
-    <t>Peanutsraffle</t>
-  </si>
-  <si>
-    <t>Playbillquilt.JPG</t>
-  </si>
-  <si>
-    <t>Playbillquilt</t>
-  </si>
-  <si>
-    <t>Playbillquilt2.JPG</t>
-  </si>
-  <si>
-    <t>Playbillquilt2</t>
-  </si>
-  <si>
-    <t>PortraitquiltMom.JPG</t>
-  </si>
-  <si>
-    <t>Portraitquiltmom</t>
-  </si>
-  <si>
-    <t>Ratatouillequilt.jpg</t>
-  </si>
-  <si>
-    <t>Ratatouillequilt</t>
-  </si>
-  <si>
-    <t>RileyCummingsgift2010.jpg</t>
-  </si>
-  <si>
-    <t>Rileycummingsgift2010</t>
-  </si>
-  <si>
-    <t>SamMinsleyMSUquilt2025.jpg</t>
-  </si>
-  <si>
-    <t>Samminsleymsuquilt2025</t>
-  </si>
-  <si>
-    <t>SesameStreetquilt.jpg</t>
-  </si>
-  <si>
-    <t>Sesamestreetquilt</t>
-  </si>
-  <si>
-    <t>StarTreckquilt.JPG</t>
-  </si>
-  <si>
-    <t>Startreckquilt</t>
-  </si>
-  <si>
-    <t>StarTrekquilt.jpg</t>
-  </si>
-  <si>
-    <t>Startrekquilt</t>
-  </si>
-  <si>
-    <t>Sunflowerqult.jpg</t>
-  </si>
-  <si>
-    <t>Sunflowerqult</t>
-  </si>
-  <si>
-    <t>Tablerunner.JPG</t>
-  </si>
-  <si>
-    <t>Tablerunner</t>
-  </si>
-  <si>
-    <t>TheVeryHungryCaterpillar.jpg</t>
-  </si>
-  <si>
-    <t>Theveryhungrycaterpillar</t>
-  </si>
-  <si>
-    <t>TropicalBirds.JPG</t>
-  </si>
-  <si>
-    <t>Tropicalbirds</t>
-  </si>
-  <si>
-    <t>Tshirtquilt for ADA.JPG</t>
-  </si>
-  <si>
-    <t>Tshirtquilt For Ada</t>
-  </si>
-  <si>
-    <t>Zebraqult.JPG</t>
-  </si>
-  <si>
-    <t>Zebraqult</t>
   </si>
 </sst>
 </file>
@@ -1177,12 +1177,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4340EA-FD21-482F-8D6B-EAA7EEEEB033}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3E5607-CA4C-4E04-8381-46D0D6074724}">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,10 +1419,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1430,10 +1430,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1452,10 +1452,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1463,10 +1463,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1474,10 +1474,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1496,10 +1496,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1507,10 +1507,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1518,10 +1518,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1529,10 +1529,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -1540,10 +1540,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -1551,10 +1551,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1562,10 +1562,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
@@ -1584,10 +1584,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
         <v>9</v>
@@ -1595,10 +1595,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" t="s">
         <v>9</v>
@@ -1606,10 +1606,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -1617,10 +1617,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>9</v>
@@ -1628,10 +1628,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
         <v>9</v>
@@ -1650,10 +1650,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -1694,10 +1694,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
@@ -1705,10 +1705,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1716,10 +1716,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -1727,10 +1727,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
         <v>9</v>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1749,10 +1749,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
         <v>9</v>

</xml_diff>